<commit_message>
Change column labels for supp table 2
</commit_message>
<xml_diff>
--- a/Data/FlowCytometerInfo.xlsx
+++ b/Data/FlowCytometerInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{C43BD7BC-606F-4542-B570-A9D3062C468B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9773C46-C5B9-8741-9B19-9D7703C6D5AD}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{C43BD7BC-606F-4542-B570-A9D3062C468B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C3B7D98-78B9-6942-9115-9CA3E07701E0}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{BE5B087C-5C52-C846-8B10-AFF54A93A08D}"/>
+    <workbookView xWindow="360" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{BE5B087C-5C52-C846-8B10-AFF54A93A08D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,6 @@
     <t>Channel</t>
   </si>
   <si>
-    <t>LysoTracker CCS Cruise</t>
-  </si>
-  <si>
-    <t>LysoTracker NES Cruise</t>
-  </si>
-  <si>
     <t>FSC</t>
   </si>
   <si>
@@ -98,16 +92,22 @@
     <t>440/50</t>
   </si>
   <si>
-    <t>Wavelength Guava (nm)</t>
-  </si>
-  <si>
-    <t>Wavelength CytPix (nm)</t>
-  </si>
-  <si>
-    <t>Culture Tests CytPix Voltage (V)</t>
-  </si>
-  <si>
-    <t>Guava Gain (Culture Tests &amp; NES FLP)</t>
+    <t>Guava Gain - Culture Tests &amp; NES FLP</t>
+  </si>
+  <si>
+    <t>Guava Gain - LysoTracker CCS</t>
+  </si>
+  <si>
+    <t>Guava Gain - LysoTracker NES</t>
+  </si>
+  <si>
+    <t>CytPix Voltage - Culture Tests</t>
+  </si>
+  <si>
+    <t>CytPix Wavelength (nm)</t>
+  </si>
+  <si>
+    <t>Guava Wavelength (nm)</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,27 +500,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>4.97</v>
@@ -537,7 +537,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2.95</v>
@@ -552,15 +552,15 @@
         <v>330</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>2.95</v>
@@ -575,15 +575,15 @@
         <v>377</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>112</v>
@@ -595,12 +595,12 @@
         <v>98.7</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>2.95</v>
@@ -615,35 +615,35 @@
         <v>280</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>354</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>